<commit_message>
A store management application created during my Java training.
</commit_message>
<xml_diff>
--- a/src/main/resources/Inventory.xlsx
+++ b/src/main/resources/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A1EE634-9CCF-4BF2-9366-5D6A42297168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E101955B-1D9F-41A1-ABC8-F5800867863B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15480" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory List" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Discontinued?</t>
   </si>
   <si>
     <t>Reorder time
@@ -43,9 +40,6 @@
     <t>1 lb package</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Frozen blueberries</t>
   </si>
   <si>
@@ -66,11 +60,28 @@
 in stock</t>
   </si>
   <si>
-    <t>Unit 
-price</t>
-  </si>
-  <si>
     <t>Product ID</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Fresh Food</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
   </si>
 </sst>
 </file>
@@ -172,7 +183,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -205,6 +216,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -218,7 +235,31 @@
     <cellStyle name="Percent" xfId="7" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -244,54 +285,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -348,6 +341,126 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Univers"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Univers"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Univers"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Univers"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -497,20 +610,20 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="2" defaultTableStyle="InventoryTable" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="InventoryTable" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="totalRow" dxfId="20"/>
-      <tableStyleElement type="firstColumn" dxfId="19"/>
-      <tableStyleElement type="lastColumn" dxfId="18"/>
-      <tableStyleElement type="firstRowStripe" dxfId="17"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="totalRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
+      <tableStyleElement type="lastColumn" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="21"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{C915C8BB-1318-46A7-9233-36C02BDC127E}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -593,17 +706,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="InventoryList" displayName="InventoryList" ref="B1:J5" headerRowDxfId="12">
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Product ID" totalsRowLabel="Total" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Unit _x000a_price" totalsRowFunction="sum" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Quantity _x000a_in stock" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reorder _x000a_level" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Reorder time_x000a_in days" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quantity in reorder" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Discontinued?" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="InventoryList" displayName="InventoryList" ref="B1:L5" headerRowDxfId="17">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Product ID" totalsRowLabel="Total" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Quantity _x000a_in stock" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{034CB113-B964-4755-9EEC-C69B4ED73509}" name="Size" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{5BA94B7A-F4CB-45B7-A2DF-0D3807859057}" name="Category" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{67D900B1-2353-4406-86D4-AC40F314441B}" name="Expiry Date" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reorder _x000a_level" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Reorder time_x000a_in days" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quantity in reorder" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -845,182 +960,198 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="17.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="2" customWidth="1"/>
-    <col min="8" max="9" width="17.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="2" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="16.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.25" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="12" customWidth="1"/>
+    <col min="8" max="9" width="20.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="2" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2"/>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E2" s="12">
+        <v>30</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="10">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="F2" s="10">
-        <v>30</v>
-      </c>
-      <c r="G2" s="10">
+      <c r="I2"/>
+      <c r="J2" s="10">
         <v>10</v>
       </c>
-      <c r="H2" s="10">
+      <c r="K2" s="10">
         <v>5</v>
       </c>
-      <c r="I2" s="10">
+      <c r="L2" s="10">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="10">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10">
         <v>8.99</v>
       </c>
-      <c r="F3" s="10">
+      <c r="E3" s="12">
         <v>12</v>
       </c>
-      <c r="G3" s="10">
+      <c r="F3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3" s="10">
         <v>5</v>
       </c>
-      <c r="H3" s="10">
+      <c r="K3" s="10">
         <v>5</v>
       </c>
-      <c r="I3" s="10">
+      <c r="L3" s="10">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="10">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10">
         <v>5.25</v>
       </c>
-      <c r="F4" s="10">
+      <c r="E4" s="12">
         <v>20</v>
       </c>
-      <c r="G4" s="10">
+      <c r="F4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4" s="10">
         <v>15</v>
       </c>
-      <c r="H4" s="10">
+      <c r="K4" s="10">
         <v>3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="L4" s="10">
         <v>50</v>
       </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="3"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Inventory ID in this column under this heading" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in this column under this heading" sqref="C1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="D1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit Price in this column under this heading" sqref="E1" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in Stock in this column under this heading" sqref="F1" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Reorder Level in this column under this heading" sqref="G1" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Reorder Time in Days in this column under this heading" sqref="H1" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in Reorder in this column under this heading" sqref="I1" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter whether the item has been discontinued in this column under this heading" sqref="J1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in this column under this heading" sqref="C1:G1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="H1:I1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit Price in this column under this heading" sqref="D1:G1" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in Stock in this column under this heading" sqref="E1:G1" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Reorder Level in this column under this heading" sqref="J1" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Reorder Time in Days in this column under this heading" sqref="K1" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in Reorder in this column under this heading" sqref="L1" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.71" right="0.71" top="0.71" bottom="0.71" header="0.5" footer="0.5"/>
@@ -1035,15 +1166,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1343,7 +1465,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -1363,15 +1485,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B6B55FC-0A09-44FF-A0E3-34C72D240197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73E471BE-D730-41C6-961C-DF2C0401B741}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1392,7 +1515,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E993646F-F722-4156-839E-6FDC5798D7F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1404,6 +1527,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B6B55FC-0A09-44FF-A0E3-34C72D240197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>